<commit_message>
changed some stuff in Diagnosis.py and Main.py to fix executable
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -585,7 +585,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -629,7 +629,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1099,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K8:AA101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
-      <selection activeCell="S50" sqref="S50:Y50"/>
+    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="P90" sqref="P90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,351 +1115,351 @@
   <sheetData>
     <row r="8" spans="11:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="11:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K9" s="61">
+      <c r="K9" s="60">
         <v>1</v>
       </c>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
       <c r="Q9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K10" s="63" t="s">
+      <c r="K10" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
       <c r="Q10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
       <c r="Q11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="78" t="s">
+      <c r="K12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77" t="s">
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="O12" s="77"/>
-      <c r="P12" s="77"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
       <c r="Q12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K13" s="67"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="70" t="s">
+      <c r="K13" s="66"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="O13" s="43"/>
-      <c r="P13" s="44"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="43"/>
       <c r="Q13" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K14" s="57"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="69" t="s">
+      <c r="K14" s="56"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="O14" s="55"/>
-      <c r="P14" s="56"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="55"/>
       <c r="Q14" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K15" s="60"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="70" t="s">
+      <c r="K15" s="59"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="O15" s="43"/>
-      <c r="P15" s="44"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="43"/>
       <c r="Q15" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K16" s="57"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="54" t="s">
+      <c r="K16" s="56"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="55"/>
-      <c r="P16" s="56"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="55"/>
       <c r="Q16" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="11:17" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K17" s="60"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="71" t="s">
+      <c r="K17" s="59"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="O17" s="72"/>
-      <c r="P17" s="73"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="72"/>
       <c r="Q17" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="11:17" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K18" s="57"/>
-      <c r="L18" s="58"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="74" t="s">
+      <c r="K18" s="56"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="O18" s="75"/>
-      <c r="P18" s="76"/>
+      <c r="O18" s="74"/>
+      <c r="P18" s="75"/>
       <c r="Q18" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K19" s="60"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="42" t="s">
+      <c r="K19" s="59"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="O19" s="43"/>
-      <c r="P19" s="44"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="43"/>
       <c r="Q19" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K20" s="57"/>
-      <c r="L20" s="58"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="54" t="s">
+      <c r="K20" s="56"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="O20" s="55"/>
-      <c r="P20" s="56"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="55"/>
       <c r="Q20" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K21" s="60"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="42" t="s">
+      <c r="K21" s="59"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="O21" s="43"/>
-      <c r="P21" s="44"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="43"/>
       <c r="Q21" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K22" s="57"/>
-      <c r="L22" s="58"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="54" t="s">
+      <c r="K22" s="56"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="O22" s="55"/>
-      <c r="P22" s="56"/>
+      <c r="O22" s="54"/>
+      <c r="P22" s="55"/>
       <c r="Q22" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K23" s="60"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="42" t="s">
+      <c r="K23" s="59"/>
+      <c r="L23" s="48"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O23" s="43"/>
-      <c r="P23" s="44"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="43"/>
       <c r="Q23" s="3">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K24" s="57"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="54" t="s">
+      <c r="K24" s="56"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="O24" s="55"/>
-      <c r="P24" s="56"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="55"/>
       <c r="Q24" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K25" s="60"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="42" t="s">
+      <c r="K25" s="59"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O25" s="43"/>
-      <c r="P25" s="44"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="43"/>
       <c r="Q25" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K26" s="57"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="54" t="s">
+      <c r="K26" s="56"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="O26" s="55"/>
-      <c r="P26" s="56"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="55"/>
       <c r="Q26" s="3">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="11:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K27" s="48" t="s">
+      <c r="K27" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="L27" s="49"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="42" t="s">
+      <c r="L27" s="48"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="44"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="43"/>
       <c r="Q27" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="11:17" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K28" s="51" t="s">
+      <c r="K28" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="52"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="45" t="s">
+      <c r="L28" s="51"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="O28" s="46"/>
-      <c r="P28" s="47"/>
+      <c r="O28" s="45"/>
+      <c r="P28" s="46"/>
       <c r="Q28" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="19:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S37" s="34">
+      <c r="S37" s="33">
         <v>1</v>
       </c>
-      <c r="T37" s="35"/>
-      <c r="U37" s="35"/>
-      <c r="V37" s="35"/>
-      <c r="W37" s="35"/>
-      <c r="X37" s="35"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="32" t="s">
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="34"/>
+      <c r="Y37" s="35"/>
+      <c r="Z37" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AA37" s="32"/>
+      <c r="AA37" s="31"/>
     </row>
     <row r="38" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S38" s="41" t="s">
+      <c r="S38" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="T38" s="30"/>
-      <c r="U38" s="30"/>
-      <c r="V38" s="30"/>
-      <c r="W38" s="30"/>
-      <c r="X38" s="30"/>
-      <c r="Y38" s="31"/>
-      <c r="Z38" s="32" t="s">
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="30"/>
+      <c r="Z38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AA38" s="32"/>
+      <c r="AA38" s="31"/>
     </row>
     <row r="39" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S39" s="29" t="s">
+      <c r="S39" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="T39" s="30"/>
-      <c r="U39" s="30"/>
-      <c r="V39" s="30"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="31"/>
-      <c r="Z39" s="32" t="s">
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="30"/>
+      <c r="Z39" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AA39" s="32"/>
+      <c r="AA39" s="31"/>
     </row>
     <row r="40" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S40" s="33" t="s">
+      <c r="S40" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="T40" s="33"/>
-      <c r="U40" s="33"/>
-      <c r="V40" s="33"/>
-      <c r="W40" s="33" t="s">
+      <c r="T40" s="32"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="32"/>
+      <c r="W40" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="X40" s="33"/>
-      <c r="Y40" s="33"/>
-      <c r="Z40" s="32"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="31"/>
       <c r="AA40" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S41" s="24"/>
-      <c r="T41" s="25"/>
-      <c r="U41" s="25"/>
-      <c r="V41" s="25"/>
-      <c r="W41" s="39" t="s">
+      <c r="S41" s="23"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="40"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="24"/>
+      <c r="Z41" s="39"/>
       <c r="AA41" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S42" s="18"/>
+      <c r="S42" s="17"/>
       <c r="T42" s="11"/>
       <c r="U42" s="11"/>
       <c r="V42" s="11"/>
@@ -1469,13 +1468,13 @@
       </c>
       <c r="X42" s="11"/>
       <c r="Y42" s="11"/>
-      <c r="Z42" s="37"/>
+      <c r="Z42" s="36"/>
       <c r="AA42" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S43" s="18"/>
+      <c r="S43" s="17"/>
       <c r="T43" s="11"/>
       <c r="U43" s="11"/>
       <c r="V43" s="11"/>
@@ -1484,7 +1483,7 @@
       </c>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
-      <c r="Z43" s="37"/>
+      <c r="Z43" s="36"/>
       <c r="AA43" s="6">
         <v>3</v>
       </c>
@@ -1501,7 +1500,7 @@
       </c>
       <c r="X44" s="11"/>
       <c r="Y44" s="11"/>
-      <c r="Z44" s="37"/>
+      <c r="Z44" s="36"/>
       <c r="AA44" s="7">
         <v>4</v>
       </c>
@@ -1518,84 +1517,84 @@
     </row>
     <row r="47" spans="19:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S48" s="34">
+      <c r="S48" s="33">
         <v>2</v>
       </c>
-      <c r="T48" s="35"/>
-      <c r="U48" s="35"/>
-      <c r="V48" s="35"/>
-      <c r="W48" s="35"/>
-      <c r="X48" s="35"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="32" t="s">
+      <c r="T48" s="34"/>
+      <c r="U48" s="34"/>
+      <c r="V48" s="34"/>
+      <c r="W48" s="34"/>
+      <c r="X48" s="34"/>
+      <c r="Y48" s="35"/>
+      <c r="Z48" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AA48" s="32"/>
+      <c r="AA48" s="31"/>
     </row>
     <row r="49" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S49" s="29" t="s">
+      <c r="S49" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="T49" s="30"/>
-      <c r="U49" s="30"/>
-      <c r="V49" s="30"/>
-      <c r="W49" s="30"/>
-      <c r="X49" s="30"/>
-      <c r="Y49" s="31"/>
-      <c r="Z49" s="32" t="s">
+      <c r="T49" s="29"/>
+      <c r="U49" s="29"/>
+      <c r="V49" s="29"/>
+      <c r="W49" s="29"/>
+      <c r="X49" s="29"/>
+      <c r="Y49" s="30"/>
+      <c r="Z49" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AA49" s="32"/>
+      <c r="AA49" s="31"/>
     </row>
     <row r="50" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S50" s="29" t="s">
+      <c r="S50" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="T50" s="30"/>
-      <c r="U50" s="30"/>
-      <c r="V50" s="30"/>
-      <c r="W50" s="30"/>
-      <c r="X50" s="30"/>
-      <c r="Y50" s="31"/>
-      <c r="Z50" s="32" t="s">
+      <c r="T50" s="29"/>
+      <c r="U50" s="29"/>
+      <c r="V50" s="29"/>
+      <c r="W50" s="29"/>
+      <c r="X50" s="29"/>
+      <c r="Y50" s="30"/>
+      <c r="Z50" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AA50" s="32"/>
+      <c r="AA50" s="31"/>
     </row>
     <row r="51" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S51" s="33" t="s">
+      <c r="S51" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="T51" s="33"/>
-      <c r="U51" s="33"/>
-      <c r="V51" s="33"/>
-      <c r="W51" s="33" t="s">
+      <c r="T51" s="32"/>
+      <c r="U51" s="32"/>
+      <c r="V51" s="32"/>
+      <c r="W51" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="X51" s="33"/>
-      <c r="Y51" s="33"/>
-      <c r="Z51" s="32"/>
+      <c r="X51" s="32"/>
+      <c r="Y51" s="32"/>
+      <c r="Z51" s="31"/>
       <c r="AA51" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S52" s="24"/>
-      <c r="T52" s="25"/>
-      <c r="U52" s="25"/>
-      <c r="V52" s="25"/>
-      <c r="W52" s="39" t="s">
+      <c r="S52" s="23"/>
+      <c r="T52" s="24"/>
+      <c r="U52" s="24"/>
+      <c r="V52" s="24"/>
+      <c r="W52" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="X52" s="25"/>
-      <c r="Y52" s="25"/>
-      <c r="Z52" s="40"/>
+      <c r="X52" s="24"/>
+      <c r="Y52" s="24"/>
+      <c r="Z52" s="39"/>
       <c r="AA52" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S53" s="18"/>
+      <c r="S53" s="17"/>
       <c r="T53" s="11"/>
       <c r="U53" s="11"/>
       <c r="V53" s="11"/>
@@ -1604,13 +1603,13 @@
       </c>
       <c r="X53" s="11"/>
       <c r="Y53" s="11"/>
-      <c r="Z53" s="37"/>
+      <c r="Z53" s="36"/>
       <c r="AA53" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S54" s="18"/>
+      <c r="S54" s="17"/>
       <c r="T54" s="11"/>
       <c r="U54" s="11"/>
       <c r="V54" s="11"/>
@@ -1619,7 +1618,7 @@
       </c>
       <c r="X54" s="11"/>
       <c r="Y54" s="11"/>
-      <c r="Z54" s="37"/>
+      <c r="Z54" s="36"/>
       <c r="AA54" s="6">
         <v>3</v>
       </c>
@@ -1628,123 +1627,123 @@
       <c r="S55" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="T55" s="38"/>
-      <c r="U55" s="38"/>
-      <c r="V55" s="38"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="37"/>
+      <c r="V55" s="37"/>
       <c r="W55" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="X55" s="19"/>
-      <c r="Y55" s="19"/>
-      <c r="Z55" s="20"/>
+      <c r="X55" s="18"/>
+      <c r="Y55" s="18"/>
+      <c r="Z55" s="19"/>
       <c r="AA55" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="19:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S58" s="34">
+      <c r="S58" s="33">
         <v>3</v>
       </c>
-      <c r="T58" s="35"/>
-      <c r="U58" s="35"/>
-      <c r="V58" s="35"/>
-      <c r="W58" s="35"/>
-      <c r="X58" s="35"/>
-      <c r="Y58" s="36"/>
-      <c r="Z58" s="32" t="s">
+      <c r="T58" s="34"/>
+      <c r="U58" s="34"/>
+      <c r="V58" s="34"/>
+      <c r="W58" s="34"/>
+      <c r="X58" s="34"/>
+      <c r="Y58" s="35"/>
+      <c r="Z58" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AA58" s="32"/>
+      <c r="AA58" s="31"/>
     </row>
     <row r="59" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S59" s="29" t="s">
+      <c r="S59" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="T59" s="30"/>
-      <c r="U59" s="30"/>
-      <c r="V59" s="30"/>
-      <c r="W59" s="30"/>
-      <c r="X59" s="30"/>
-      <c r="Y59" s="31"/>
-      <c r="Z59" s="32" t="s">
+      <c r="T59" s="29"/>
+      <c r="U59" s="29"/>
+      <c r="V59" s="29"/>
+      <c r="W59" s="29"/>
+      <c r="X59" s="29"/>
+      <c r="Y59" s="30"/>
+      <c r="Z59" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AA59" s="32"/>
+      <c r="AA59" s="31"/>
     </row>
     <row r="60" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S60" s="29" t="s">
+      <c r="S60" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="T60" s="30"/>
-      <c r="U60" s="30"/>
-      <c r="V60" s="30"/>
-      <c r="W60" s="30"/>
-      <c r="X60" s="30"/>
-      <c r="Y60" s="31"/>
-      <c r="Z60" s="32" t="s">
+      <c r="T60" s="29"/>
+      <c r="U60" s="29"/>
+      <c r="V60" s="29"/>
+      <c r="W60" s="29"/>
+      <c r="X60" s="29"/>
+      <c r="Y60" s="30"/>
+      <c r="Z60" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AA60" s="32"/>
+      <c r="AA60" s="31"/>
     </row>
     <row r="61" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S61" s="33" t="s">
+      <c r="S61" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="T61" s="33"/>
-      <c r="U61" s="33"/>
-      <c r="V61" s="33"/>
-      <c r="W61" s="33" t="s">
+      <c r="T61" s="32"/>
+      <c r="U61" s="32"/>
+      <c r="V61" s="32"/>
+      <c r="W61" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="X61" s="33"/>
-      <c r="Y61" s="33"/>
-      <c r="Z61" s="32"/>
+      <c r="X61" s="32"/>
+      <c r="Y61" s="32"/>
+      <c r="Z61" s="31"/>
       <c r="AA61" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="62" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S62" s="24"/>
-      <c r="T62" s="25"/>
-      <c r="U62" s="25"/>
-      <c r="V62" s="25"/>
-      <c r="W62" s="26" t="s">
+      <c r="S62" s="23"/>
+      <c r="T62" s="24"/>
+      <c r="U62" s="24"/>
+      <c r="V62" s="24"/>
+      <c r="W62" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="X62" s="27"/>
-      <c r="Y62" s="27"/>
-      <c r="Z62" s="28"/>
+      <c r="X62" s="26"/>
+      <c r="Y62" s="26"/>
+      <c r="Z62" s="27"/>
       <c r="AA62" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S63" s="18"/>
+      <c r="S63" s="17"/>
       <c r="T63" s="11"/>
       <c r="U63" s="11"/>
       <c r="V63" s="11"/>
       <c r="W63" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="X63" s="19"/>
-      <c r="Y63" s="19"/>
-      <c r="Z63" s="20"/>
+      <c r="X63" s="18"/>
+      <c r="Y63" s="18"/>
+      <c r="Z63" s="19"/>
       <c r="AA63" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S64" s="18"/>
+      <c r="S64" s="17"/>
       <c r="T64" s="11"/>
       <c r="U64" s="11"/>
       <c r="V64" s="11"/>
       <c r="W64" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="X64" s="19"/>
-      <c r="Y64" s="19"/>
-      <c r="Z64" s="20"/>
+      <c r="X64" s="18"/>
+      <c r="Y64" s="18"/>
+      <c r="Z64" s="19"/>
       <c r="AA64" s="6">
         <v>3</v>
       </c>
@@ -1757,24 +1756,24 @@
       <c r="W65" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="X65" s="19"/>
-      <c r="Y65" s="19"/>
-      <c r="Z65" s="20"/>
+      <c r="X65" s="18"/>
+      <c r="Y65" s="18"/>
+      <c r="Z65" s="19"/>
       <c r="AA65" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="19:27" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S66" s="18"/>
+      <c r="S66" s="17"/>
       <c r="T66" s="11"/>
       <c r="U66" s="11"/>
       <c r="V66" s="11"/>
-      <c r="W66" s="21" t="s">
+      <c r="W66" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="X66" s="22"/>
-      <c r="Y66" s="22"/>
-      <c r="Z66" s="23"/>
+      <c r="X66" s="21"/>
+      <c r="Y66" s="21"/>
+      <c r="Z66" s="22"/>
       <c r="AA66" s="9">
         <v>5</v>
       </c>
@@ -1784,27 +1783,27 @@
       <c r="T67" s="11"/>
       <c r="U67" s="11"/>
       <c r="V67" s="11"/>
-      <c r="W67" s="21" t="s">
+      <c r="W67" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="X67" s="22"/>
-      <c r="Y67" s="22"/>
-      <c r="Z67" s="23"/>
+      <c r="X67" s="21"/>
+      <c r="Y67" s="21"/>
+      <c r="Z67" s="22"/>
       <c r="AA67" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="68" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S68" s="18"/>
+      <c r="S68" s="17"/>
       <c r="T68" s="11"/>
       <c r="U68" s="11"/>
       <c r="V68" s="11"/>
       <c r="W68" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="X68" s="19"/>
-      <c r="Y68" s="19"/>
-      <c r="Z68" s="20"/>
+      <c r="X68" s="18"/>
+      <c r="Y68" s="18"/>
+      <c r="Z68" s="19"/>
       <c r="AA68" s="6">
         <v>7</v>
       </c>
@@ -1814,18 +1813,18 @@
       <c r="T69" s="11"/>
       <c r="U69" s="11"/>
       <c r="V69" s="11"/>
-      <c r="W69" s="21" t="s">
+      <c r="W69" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="X69" s="22"/>
-      <c r="Y69" s="22"/>
-      <c r="Z69" s="23"/>
+      <c r="X69" s="21"/>
+      <c r="Y69" s="21"/>
+      <c r="Z69" s="22"/>
       <c r="AA69" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="70" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S70" s="18"/>
+      <c r="S70" s="17"/>
       <c r="T70" s="11"/>
       <c r="U70" s="11"/>
       <c r="V70" s="11"/>
@@ -1855,7 +1854,7 @@
       </c>
     </row>
     <row r="72" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S72" s="18"/>
+      <c r="S72" s="17"/>
       <c r="T72" s="11"/>
       <c r="U72" s="11"/>
       <c r="V72" s="11"/>
@@ -1885,7 +1884,7 @@
       </c>
     </row>
     <row r="74" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S74" s="18"/>
+      <c r="S74" s="17"/>
       <c r="T74" s="11"/>
       <c r="U74" s="11"/>
       <c r="V74" s="11"/>
@@ -1950,108 +1949,108 @@
     </row>
     <row r="79" spans="19:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S80" s="34">
+      <c r="S80" s="33">
         <v>4</v>
       </c>
-      <c r="T80" s="35"/>
-      <c r="U80" s="35"/>
-      <c r="V80" s="35"/>
-      <c r="W80" s="35"/>
-      <c r="X80" s="35"/>
-      <c r="Y80" s="36"/>
-      <c r="Z80" s="32" t="s">
+      <c r="T80" s="34"/>
+      <c r="U80" s="34"/>
+      <c r="V80" s="34"/>
+      <c r="W80" s="34"/>
+      <c r="X80" s="34"/>
+      <c r="Y80" s="35"/>
+      <c r="Z80" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AA80" s="32"/>
+      <c r="AA80" s="31"/>
     </row>
     <row r="81" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S81" s="29" t="s">
+      <c r="S81" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="T81" s="30"/>
-      <c r="U81" s="30"/>
-      <c r="V81" s="30"/>
-      <c r="W81" s="30"/>
-      <c r="X81" s="30"/>
-      <c r="Y81" s="31"/>
-      <c r="Z81" s="32" t="s">
+      <c r="T81" s="29"/>
+      <c r="U81" s="29"/>
+      <c r="V81" s="29"/>
+      <c r="W81" s="29"/>
+      <c r="X81" s="29"/>
+      <c r="Y81" s="30"/>
+      <c r="Z81" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AA81" s="32"/>
+      <c r="AA81" s="31"/>
     </row>
     <row r="82" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S82" s="29" t="s">
+      <c r="S82" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="T82" s="30"/>
-      <c r="U82" s="30"/>
-      <c r="V82" s="30"/>
-      <c r="W82" s="30"/>
-      <c r="X82" s="30"/>
-      <c r="Y82" s="31"/>
-      <c r="Z82" s="32" t="s">
+      <c r="T82" s="29"/>
+      <c r="U82" s="29"/>
+      <c r="V82" s="29"/>
+      <c r="W82" s="29"/>
+      <c r="X82" s="29"/>
+      <c r="Y82" s="30"/>
+      <c r="Z82" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AA82" s="32"/>
+      <c r="AA82" s="31"/>
     </row>
     <row r="83" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S83" s="33" t="s">
+      <c r="S83" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="T83" s="33"/>
-      <c r="U83" s="33"/>
-      <c r="V83" s="33"/>
-      <c r="W83" s="33" t="s">
+      <c r="T83" s="32"/>
+      <c r="U83" s="32"/>
+      <c r="V83" s="32"/>
+      <c r="W83" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="X83" s="33"/>
-      <c r="Y83" s="33"/>
-      <c r="Z83" s="32"/>
+      <c r="X83" s="32"/>
+      <c r="Y83" s="32"/>
+      <c r="Z83" s="31"/>
       <c r="AA83" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="84" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S84" s="24"/>
-      <c r="T84" s="25"/>
-      <c r="U84" s="25"/>
-      <c r="V84" s="25"/>
-      <c r="W84" s="26" t="s">
+      <c r="S84" s="23"/>
+      <c r="T84" s="24"/>
+      <c r="U84" s="24"/>
+      <c r="V84" s="24"/>
+      <c r="W84" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="X84" s="27"/>
-      <c r="Y84" s="27"/>
-      <c r="Z84" s="28"/>
+      <c r="X84" s="26"/>
+      <c r="Y84" s="26"/>
+      <c r="Z84" s="27"/>
       <c r="AA84" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S85" s="18"/>
+      <c r="S85" s="17"/>
       <c r="T85" s="11"/>
       <c r="U85" s="11"/>
       <c r="V85" s="11"/>
       <c r="W85" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="X85" s="19"/>
-      <c r="Y85" s="19"/>
-      <c r="Z85" s="20"/>
+      <c r="X85" s="18"/>
+      <c r="Y85" s="18"/>
+      <c r="Z85" s="19"/>
       <c r="AA85" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S86" s="18"/>
+      <c r="S86" s="17"/>
       <c r="T86" s="11"/>
       <c r="U86" s="11"/>
       <c r="V86" s="11"/>
       <c r="W86" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="X86" s="19"/>
-      <c r="Y86" s="19"/>
-      <c r="Z86" s="20"/>
+      <c r="X86" s="18"/>
+      <c r="Y86" s="18"/>
+      <c r="Z86" s="19"/>
       <c r="AA86" s="6">
         <v>3</v>
       </c>
@@ -2064,24 +2063,24 @@
       <c r="W87" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="X87" s="19"/>
-      <c r="Y87" s="19"/>
-      <c r="Z87" s="20"/>
+      <c r="X87" s="18"/>
+      <c r="Y87" s="18"/>
+      <c r="Z87" s="19"/>
       <c r="AA87" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="88" spans="19:27" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S88" s="18"/>
+      <c r="S88" s="17"/>
       <c r="T88" s="11"/>
       <c r="U88" s="11"/>
       <c r="V88" s="11"/>
-      <c r="W88" s="21" t="s">
+      <c r="W88" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="X88" s="22"/>
-      <c r="Y88" s="22"/>
-      <c r="Z88" s="23"/>
+      <c r="X88" s="21"/>
+      <c r="Y88" s="21"/>
+      <c r="Z88" s="22"/>
       <c r="AA88" s="9">
         <v>5</v>
       </c>
@@ -2091,27 +2090,27 @@
       <c r="T89" s="11"/>
       <c r="U89" s="11"/>
       <c r="V89" s="11"/>
-      <c r="W89" s="21" t="s">
+      <c r="W89" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="X89" s="22"/>
-      <c r="Y89" s="22"/>
-      <c r="Z89" s="23"/>
+      <c r="X89" s="21"/>
+      <c r="Y89" s="21"/>
+      <c r="Z89" s="22"/>
       <c r="AA89" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="90" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S90" s="18"/>
+      <c r="S90" s="17"/>
       <c r="T90" s="11"/>
       <c r="U90" s="11"/>
       <c r="V90" s="11"/>
       <c r="W90" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="X90" s="19"/>
-      <c r="Y90" s="19"/>
-      <c r="Z90" s="20"/>
+      <c r="X90" s="18"/>
+      <c r="Y90" s="18"/>
+      <c r="Z90" s="19"/>
       <c r="AA90" s="6">
         <v>7</v>
       </c>
@@ -2121,18 +2120,18 @@
       <c r="T91" s="11"/>
       <c r="U91" s="11"/>
       <c r="V91" s="11"/>
-      <c r="W91" s="21" t="s">
+      <c r="W91" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="X91" s="22"/>
-      <c r="Y91" s="22"/>
-      <c r="Z91" s="23"/>
+      <c r="X91" s="21"/>
+      <c r="Y91" s="21"/>
+      <c r="Z91" s="22"/>
       <c r="AA91" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="92" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S92" s="18"/>
+      <c r="S92" s="17"/>
       <c r="T92" s="11"/>
       <c r="U92" s="11"/>
       <c r="V92" s="11"/>
@@ -2162,7 +2161,7 @@
       </c>
     </row>
     <row r="94" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S94" s="18"/>
+      <c r="S94" s="17"/>
       <c r="T94" s="11"/>
       <c r="U94" s="11"/>
       <c r="V94" s="11"/>
@@ -2192,7 +2191,7 @@
       </c>
     </row>
     <row r="96" spans="19:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S96" s="18"/>
+      <c r="S96" s="17"/>
       <c r="T96" s="11"/>
       <c r="U96" s="11"/>
       <c r="V96" s="11"/>
@@ -2273,17 +2272,17 @@
       </c>
     </row>
     <row r="101" spans="19:27" x14ac:dyDescent="0.25">
-      <c r="S101" s="17"/>
-      <c r="T101" s="17"/>
-      <c r="U101" s="17"/>
-      <c r="V101" s="17"/>
-      <c r="W101" s="17"/>
-      <c r="X101" s="17"/>
-      <c r="Y101" s="17"/>
-      <c r="Z101" s="17"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="153">
+  <mergeCells count="151">
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="N21:P21"/>
     <mergeCell ref="K9:P9"/>
@@ -2429,8 +2428,6 @@
     <mergeCell ref="W99:Z99"/>
     <mergeCell ref="S100:V100"/>
     <mergeCell ref="W100:Z100"/>
-    <mergeCell ref="S101:V101"/>
-    <mergeCell ref="W101:Z101"/>
     <mergeCell ref="S96:V96"/>
     <mergeCell ref="W96:Z96"/>
     <mergeCell ref="S97:V97"/>

</xml_diff>